<commit_message>
Adição ponto 2 lista 1 - interpolação linear
</commit_message>
<xml_diff>
--- a/MQI2104/lista1.xlsx
+++ b/MQI2104/lista1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juan_\MuGoL\E-learning\Matlab\MQI2104\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A64CF97C-ED49-4A95-BEDE-248C4EC28C1B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60F78BAD-226D-42CF-BD20-29153FD67BD9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="828" yWindow="-108" windowWidth="22320" windowHeight="13176" xr2:uid="{B96B6BAE-0F66-4A3B-BB89-80284C847D59}"/>
+    <workbookView xWindow="2052" yWindow="1116" windowWidth="16584" windowHeight="9420" xr2:uid="{B96B6BAE-0F66-4A3B-BB89-80284C847D59}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t>d (cm)</t>
   </si>
@@ -65,6 +65,40 @@
   <si>
     <t>Tensão 
 Media</t>
+  </si>
+  <si>
+    <t>yi</t>
+  </si>
+  <si>
+    <t>x(k)</t>
+  </si>
+  <si>
+    <t>y(k)</t>
+  </si>
+  <si>
+    <t>x(k+1)</t>
+  </si>
+  <si>
+    <t>y(k+1)</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>xi</t>
+  </si>
+  <si>
+    <t>Ponto inicial</t>
+  </si>
+  <si>
+    <t>Ponto Final</t>
+  </si>
+  <si>
+    <t>Tensão 
+em campo</t>
+  </si>
+  <si>
+    <t>Distâncias correspondentes as Tensões em campo</t>
   </si>
 </sst>
 </file>
@@ -232,7 +266,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -246,6 +280,14 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -258,12 +300,25 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -281,6 +336,1090 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-BR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Planilha1!$A$3:$A$35</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="33"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>6.5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>7.5</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>8.5</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>9.5</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>10.5</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Planilha1!$L$3:$L$35</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="33"/>
+                <c:pt idx="0">
+                  <c:v>1.2000000000000003E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.2109000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.8544</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.1203000000000003</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.2173000000000003</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.226</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.1112000000000002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.9189000000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.7707000000000002</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.6473000000000002</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.4994999999999998</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.3721000000000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.2754999999999999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.1695999999999998</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.0760000000000001</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.99680000000000002</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.92379999999999995</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.84619999999999995</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.74409999999999998</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.71819999999999995</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.64649999999999996</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.59210000000000007</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.51920000000000011</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.44290000000000002</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.35810000000000003</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.33360000000000001</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.27430000000000004</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.21929999999999997</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.20200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.17099999999999999</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.1394</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.10269999999999999</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.12039999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-CE3B-40F5-8B9B-492D2B179463}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1095292783"/>
+        <c:axId val="1094799743"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1095292783"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1094799743"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1094799743"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.0000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1095292783"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-BR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>468630</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>175260</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>163830</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0F073DF2-DB03-42AA-B756-497F1B8AC4EE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -580,74 +1719,113 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8221740B-00B1-4E0E-A408-46F8536BDE22}">
-  <dimension ref="A1:L35"/>
+  <dimension ref="A1:T35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="12" max="12" width="13.6640625" customWidth="1"/>
+    <col min="13" max="13" width="10.33203125" customWidth="1"/>
+    <col min="19" max="19" width="23.109375" customWidth="1"/>
+    <col min="20" max="20" width="2.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:20" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="9" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="9" t="s">
         <v>9</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="K1" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="12" t="s">
+      <c r="L1" s="8" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="6"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
+      <c r="M1" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="N1" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="O1" s="17"/>
+      <c r="P1" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q1" s="17"/>
+      <c r="S1" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="T1" s="19"/>
+    </row>
+    <row r="2" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
       <c r="H2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="6"/>
+      <c r="I2" s="10"/>
       <c r="J2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="8"/>
-      <c r="L2" s="12"/>
-    </row>
-    <row r="3" spans="1:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K2" s="12"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="N2" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="O2" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="P2" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q2" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="R2" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="S2" s="16" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3">
         <v>0</v>
       </c>
@@ -678,15 +1856,38 @@
       <c r="J3" s="4">
         <v>-3.9E-2</v>
       </c>
-      <c r="K3" s="9">
+      <c r="K3" s="5">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="L3" s="11">
+      <c r="L3" s="7">
         <f>AVERAGE(B3,C3,D3,E3,F3,G3,H3,I3,J3,K3)</f>
         <v>1.2000000000000003E-3</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="M3" s="14">
+        <v>0.15</v>
+      </c>
+      <c r="N3" s="14">
+        <v>0</v>
+      </c>
+      <c r="O3" s="14">
+        <v>0</v>
+      </c>
+      <c r="P3" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="Q3" s="14">
+        <v>1.2109000000000001</v>
+      </c>
+      <c r="R3" s="15">
+        <f>(Q3-O3)/(P3-N3)</f>
+        <v>4.8436000000000003</v>
+      </c>
+      <c r="S3" s="15">
+        <f>((M3-O3)/R3)+N3</f>
+        <v>3.0968700966223468E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3">
         <v>0.25</v>
       </c>
@@ -717,15 +1918,38 @@
       <c r="J4" s="4">
         <v>1.2609999999999999</v>
       </c>
-      <c r="K4" s="9">
+      <c r="K4" s="5">
         <v>1.236</v>
       </c>
-      <c r="L4" s="10">
+      <c r="L4" s="6">
         <f t="shared" ref="L4:L35" si="0">AVERAGE(B4,C4,D4,E4,F4,G4,H4,I4,J4,K4)</f>
         <v>1.2109000000000001</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="M4" s="14">
+        <v>0.67300000000000004</v>
+      </c>
+      <c r="N4" s="14">
+        <v>0</v>
+      </c>
+      <c r="O4" s="14">
+        <v>0</v>
+      </c>
+      <c r="P4" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="Q4" s="14">
+        <v>1.2109000000000001</v>
+      </c>
+      <c r="R4" s="15">
+        <f t="shared" ref="R4:R7" si="1">(Q4-O4)/(P4-N4)</f>
+        <v>4.8436000000000003</v>
+      </c>
+      <c r="S4" s="15">
+        <f t="shared" ref="S4:S7" si="2">((M4-O4)/R4)+N4</f>
+        <v>0.13894623833512262</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="3">
         <v>0.5</v>
       </c>
@@ -756,15 +1980,38 @@
       <c r="J5" s="4">
         <v>1.871</v>
       </c>
-      <c r="K5" s="9">
+      <c r="K5" s="5">
         <v>1.8280000000000001</v>
       </c>
-      <c r="L5" s="10">
+      <c r="L5" s="6">
         <f t="shared" si="0"/>
         <v>1.8544</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="M5" s="14">
+        <v>1.52</v>
+      </c>
+      <c r="N5" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="O5" s="14">
+        <v>1.2109000000000001</v>
+      </c>
+      <c r="P5" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="Q5" s="14">
+        <v>1.8544</v>
+      </c>
+      <c r="R5" s="15">
+        <f t="shared" si="1"/>
+        <v>2.5739999999999998</v>
+      </c>
+      <c r="S5" s="15">
+        <f t="shared" si="2"/>
+        <v>0.37008547008547005</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3">
         <v>0.75</v>
       </c>
@@ -795,15 +2042,38 @@
       <c r="J6" s="4">
         <v>2.1309999999999998</v>
       </c>
-      <c r="K6" s="9">
+      <c r="K6" s="5">
         <v>2.149</v>
       </c>
-      <c r="L6" s="10">
+      <c r="L6" s="6">
         <f t="shared" si="0"/>
         <v>2.1203000000000003</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="M6" s="14">
+        <v>1.82</v>
+      </c>
+      <c r="N6" s="14">
+        <v>0.25</v>
+      </c>
+      <c r="O6" s="14">
+        <v>1.2109000000000001</v>
+      </c>
+      <c r="P6" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="Q6" s="14">
+        <v>1.8544</v>
+      </c>
+      <c r="R6" s="15">
+        <f t="shared" si="1"/>
+        <v>2.5739999999999998</v>
+      </c>
+      <c r="S6" s="15">
+        <f t="shared" si="2"/>
+        <v>0.48663558663558665</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="3">
         <v>1</v>
       </c>
@@ -834,15 +2104,38 @@
       <c r="J7" s="4">
         <v>2.2559999999999998</v>
       </c>
-      <c r="K7" s="9">
+      <c r="K7" s="5">
         <v>2.234</v>
       </c>
-      <c r="L7" s="10">
+      <c r="L7" s="6">
         <f t="shared" si="0"/>
         <v>2.2173000000000003</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="M7" s="14">
+        <v>2.2050000000000001</v>
+      </c>
+      <c r="N7" s="14">
+        <v>1.5</v>
+      </c>
+      <c r="O7" s="14">
+        <v>2.226</v>
+      </c>
+      <c r="P7" s="14">
+        <v>2</v>
+      </c>
+      <c r="Q7" s="14">
+        <v>2.1112000000000002</v>
+      </c>
+      <c r="R7" s="15">
+        <f t="shared" si="1"/>
+        <v>-0.22959999999999958</v>
+      </c>
+      <c r="S7" s="15">
+        <f t="shared" si="2"/>
+        <v>1.5914634146341462</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="3">
         <v>1.5</v>
       </c>
@@ -873,15 +2166,15 @@
       <c r="J8" s="4">
         <v>2.2040000000000002</v>
       </c>
-      <c r="K8" s="9">
+      <c r="K8" s="5">
         <v>2.2400000000000002</v>
       </c>
-      <c r="L8" s="10">
+      <c r="L8" s="6">
         <f t="shared" si="0"/>
         <v>2.226</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="3">
         <v>2</v>
       </c>
@@ -912,15 +2205,15 @@
       <c r="J9" s="4">
         <v>2.0609999999999999</v>
       </c>
-      <c r="K9" s="9">
+      <c r="K9" s="5">
         <v>2.125</v>
       </c>
-      <c r="L9" s="10">
+      <c r="L9" s="6">
         <f t="shared" si="0"/>
         <v>2.1112000000000002</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="3">
         <v>2.5</v>
       </c>
@@ -951,15 +2244,15 @@
       <c r="J10" s="4">
         <v>1.9239999999999999</v>
       </c>
-      <c r="K10" s="9">
+      <c r="K10" s="5">
         <v>1.9570000000000001</v>
       </c>
-      <c r="L10" s="10">
+      <c r="L10" s="6">
         <f t="shared" si="0"/>
         <v>1.9189000000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="3">
         <v>3</v>
       </c>
@@ -990,15 +2283,15 @@
       <c r="J11" s="4">
         <v>1.8320000000000001</v>
       </c>
-      <c r="K11" s="9">
+      <c r="K11" s="5">
         <v>1.756</v>
       </c>
-      <c r="L11" s="10">
+      <c r="L11" s="6">
         <f t="shared" si="0"/>
         <v>1.7707000000000002</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="3">
         <v>3.5</v>
       </c>
@@ -1029,15 +2322,15 @@
       <c r="J12" s="4">
         <v>1.629</v>
       </c>
-      <c r="K12" s="9">
+      <c r="K12" s="5">
         <v>1.6160000000000001</v>
       </c>
-      <c r="L12" s="10">
+      <c r="L12" s="6">
         <f t="shared" si="0"/>
         <v>1.6473000000000002</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="3">
         <v>4</v>
       </c>
@@ -1068,15 +2361,15 @@
       <c r="J13" s="4">
         <v>1.4850000000000001</v>
       </c>
-      <c r="K13" s="9">
+      <c r="K13" s="5">
         <v>1.458</v>
       </c>
-      <c r="L13" s="10">
+      <c r="L13" s="6">
         <f t="shared" si="0"/>
         <v>1.4994999999999998</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="3">
         <v>4.5</v>
       </c>
@@ -1107,15 +2400,15 @@
       <c r="J14" s="4">
         <v>1.337</v>
       </c>
-      <c r="K14" s="9">
+      <c r="K14" s="5">
         <v>1.4259999999999999</v>
       </c>
-      <c r="L14" s="10">
+      <c r="L14" s="6">
         <f t="shared" si="0"/>
         <v>1.3721000000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="3">
         <v>5</v>
       </c>
@@ -1146,15 +2439,15 @@
       <c r="J15" s="4">
         <v>1.216</v>
       </c>
-      <c r="K15" s="9">
+      <c r="K15" s="5">
         <v>1.266</v>
       </c>
-      <c r="L15" s="10">
+      <c r="L15" s="6">
         <f t="shared" si="0"/>
         <v>1.2754999999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="3">
         <v>5.5</v>
       </c>
@@ -1185,10 +2478,10 @@
       <c r="J16" s="4">
         <v>1.163</v>
       </c>
-      <c r="K16" s="9">
+      <c r="K16" s="5">
         <v>1.133</v>
       </c>
-      <c r="L16" s="10">
+      <c r="L16" s="6">
         <f t="shared" si="0"/>
         <v>1.1695999999999998</v>
       </c>
@@ -1224,10 +2517,10 @@
       <c r="J17" s="4">
         <v>1.113</v>
       </c>
-      <c r="K17" s="9">
+      <c r="K17" s="5">
         <v>1.097</v>
       </c>
-      <c r="L17" s="10">
+      <c r="L17" s="6">
         <f t="shared" si="0"/>
         <v>1.0760000000000001</v>
       </c>
@@ -1263,10 +2556,10 @@
       <c r="J18" s="4">
         <v>1.034</v>
       </c>
-      <c r="K18" s="9">
+      <c r="K18" s="5">
         <v>0.95499999999999996</v>
       </c>
-      <c r="L18" s="10">
+      <c r="L18" s="6">
         <f t="shared" si="0"/>
         <v>0.99680000000000002</v>
       </c>
@@ -1302,10 +2595,10 @@
       <c r="J19" s="4">
         <v>0.92300000000000004</v>
       </c>
-      <c r="K19" s="9">
+      <c r="K19" s="5">
         <v>0.91700000000000004</v>
       </c>
-      <c r="L19" s="10">
+      <c r="L19" s="6">
         <f t="shared" si="0"/>
         <v>0.92379999999999995</v>
       </c>
@@ -1341,10 +2634,10 @@
       <c r="J20" s="4">
         <v>0.80900000000000005</v>
       </c>
-      <c r="K20" s="9">
+      <c r="K20" s="5">
         <v>0.89100000000000001</v>
       </c>
-      <c r="L20" s="10">
+      <c r="L20" s="6">
         <f t="shared" si="0"/>
         <v>0.84619999999999995</v>
       </c>
@@ -1380,10 +2673,10 @@
       <c r="J21" s="4">
         <v>0.73899999999999999</v>
       </c>
-      <c r="K21" s="9">
+      <c r="K21" s="5">
         <v>0.79700000000000004</v>
       </c>
-      <c r="L21" s="10">
+      <c r="L21" s="6">
         <f t="shared" si="0"/>
         <v>0.74409999999999998</v>
       </c>
@@ -1419,10 +2712,10 @@
       <c r="J22" s="4">
         <v>0.70899999999999996</v>
       </c>
-      <c r="K22" s="9">
+      <c r="K22" s="5">
         <v>0.68600000000000005</v>
       </c>
-      <c r="L22" s="10">
+      <c r="L22" s="6">
         <f t="shared" si="0"/>
         <v>0.71819999999999995</v>
       </c>
@@ -1458,10 +2751,10 @@
       <c r="J23" s="4">
         <v>0.67800000000000005</v>
       </c>
-      <c r="K23" s="9">
+      <c r="K23" s="5">
         <v>0.63100000000000001</v>
       </c>
-      <c r="L23" s="10">
+      <c r="L23" s="6">
         <f t="shared" si="0"/>
         <v>0.64649999999999996</v>
       </c>
@@ -1497,10 +2790,10 @@
       <c r="J24" s="4">
         <v>0.627</v>
       </c>
-      <c r="K24" s="9">
+      <c r="K24" s="5">
         <v>0.67</v>
       </c>
-      <c r="L24" s="10">
+      <c r="L24" s="6">
         <f t="shared" si="0"/>
         <v>0.59210000000000007</v>
       </c>
@@ -1536,10 +2829,10 @@
       <c r="J25" s="4">
         <v>0.44</v>
       </c>
-      <c r="K25" s="9">
+      <c r="K25" s="5">
         <v>0.52700000000000002</v>
       </c>
-      <c r="L25" s="10">
+      <c r="L25" s="6">
         <f t="shared" si="0"/>
         <v>0.51920000000000011</v>
       </c>
@@ -1575,10 +2868,10 @@
       <c r="J26" s="4">
         <v>0.44800000000000001</v>
       </c>
-      <c r="K26" s="9">
+      <c r="K26" s="5">
         <v>0.46400000000000002</v>
       </c>
-      <c r="L26" s="10">
+      <c r="L26" s="6">
         <f t="shared" si="0"/>
         <v>0.44290000000000002</v>
       </c>
@@ -1614,10 +2907,10 @@
       <c r="J27" s="4">
         <v>0.33600000000000002</v>
       </c>
-      <c r="K27" s="9">
+      <c r="K27" s="5">
         <v>0.39400000000000002</v>
       </c>
-      <c r="L27" s="10">
+      <c r="L27" s="6">
         <f t="shared" si="0"/>
         <v>0.35810000000000003</v>
       </c>
@@ -1653,10 +2946,10 @@
       <c r="J28" s="4">
         <v>0.29799999999999999</v>
       </c>
-      <c r="K28" s="9">
+      <c r="K28" s="5">
         <v>0.36099999999999999</v>
       </c>
-      <c r="L28" s="10">
+      <c r="L28" s="6">
         <f t="shared" si="0"/>
         <v>0.33360000000000001</v>
       </c>
@@ -1692,10 +2985,10 @@
       <c r="J29" s="4">
         <v>0.34599999999999997</v>
       </c>
-      <c r="K29" s="9">
+      <c r="K29" s="5">
         <v>0.27800000000000002</v>
       </c>
-      <c r="L29" s="10">
+      <c r="L29" s="6">
         <f t="shared" si="0"/>
         <v>0.27430000000000004</v>
       </c>
@@ -1731,10 +3024,10 @@
       <c r="J30" s="4">
         <v>0.191</v>
       </c>
-      <c r="K30" s="9">
+      <c r="K30" s="5">
         <v>0.24199999999999999</v>
       </c>
-      <c r="L30" s="10">
+      <c r="L30" s="6">
         <f t="shared" si="0"/>
         <v>0.21929999999999997</v>
       </c>
@@ -1770,10 +3063,10 @@
       <c r="J31" s="4">
         <v>0.115</v>
       </c>
-      <c r="K31" s="9">
+      <c r="K31" s="5">
         <v>0.20499999999999999</v>
       </c>
-      <c r="L31" s="10">
+      <c r="L31" s="6">
         <f t="shared" si="0"/>
         <v>0.20200000000000001</v>
       </c>
@@ -1809,10 +3102,10 @@
       <c r="J32" s="4">
         <v>0.16800000000000001</v>
       </c>
-      <c r="K32" s="9">
+      <c r="K32" s="5">
         <v>0.28100000000000003</v>
       </c>
-      <c r="L32" s="10">
+      <c r="L32" s="6">
         <f t="shared" si="0"/>
         <v>0.17099999999999999</v>
       </c>
@@ -1848,10 +3141,10 @@
       <c r="J33" s="4">
         <v>0.129</v>
       </c>
-      <c r="K33" s="9">
+      <c r="K33" s="5">
         <v>0.17399999999999999</v>
       </c>
-      <c r="L33" s="10">
+      <c r="L33" s="6">
         <f t="shared" si="0"/>
         <v>0.1394</v>
       </c>
@@ -1887,10 +3180,10 @@
       <c r="J34" s="4">
         <v>9.5000000000000001E-2</v>
       </c>
-      <c r="K34" s="9">
+      <c r="K34" s="5">
         <v>7.3999999999999996E-2</v>
       </c>
-      <c r="L34" s="10">
+      <c r="L34" s="6">
         <f t="shared" si="0"/>
         <v>0.10269999999999999</v>
       </c>
@@ -1926,16 +3219,19 @@
       <c r="J35" s="4">
         <v>0.13500000000000001</v>
       </c>
-      <c r="K35" s="9">
+      <c r="K35" s="5">
         <v>4.1000000000000002E-2</v>
       </c>
-      <c r="L35" s="10">
+      <c r="L35" s="6">
         <f t="shared" si="0"/>
         <v>0.12039999999999999</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="13">
+    <mergeCell ref="N1:O1"/>
+    <mergeCell ref="P1:Q1"/>
+    <mergeCell ref="S1:T1"/>
     <mergeCell ref="L1:L2"/>
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="I1:I2"/>
@@ -1949,5 +3245,6 @@
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
correcao ponto 2 da lista 1
</commit_message>
<xml_diff>
--- a/MQI2104/lista1.xlsx
+++ b/MQI2104/lista1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juan_\MuGoL\E-learning\Matlab\MQI2104\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sammy\Desktop\matlabJuan\matlab\MQI2104\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60F78BAD-226D-42CF-BD20-29153FD67BD9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64419767-DF8F-4D53-80F1-73B55E36AD77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2052" yWindow="1116" windowWidth="16584" windowHeight="9420" xr2:uid="{B96B6BAE-0F66-4A3B-BB89-80284C847D59}"/>
+    <workbookView xWindow="15" yWindow="1320" windowWidth="8490" windowHeight="10200" xr2:uid="{B96B6BAE-0F66-4A3B-BB89-80284C847D59}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -105,9 +105,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
+    <numFmt numFmtId="166" formatCode="0.000000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -266,7 +267,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -285,6 +286,27 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -300,26 +322,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -341,7 +346,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="pt-BR"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -378,7 +383,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="pt-BR"/>
+          <a:endParaRPr lang="es-BR"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -704,7 +709,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pt-BR"/>
+            <a:endParaRPr lang="es-BR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1094799743"/>
@@ -766,7 +771,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pt-BR"/>
+            <a:endParaRPr lang="es-BR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1095292783"/>
@@ -814,7 +819,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="pt-BR"/>
+      <a:endParaRPr lang="es-BR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1423,7 +1428,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1721,111 +1726,111 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8221740B-00B1-4E0E-A408-46F8536BDE22}">
   <dimension ref="A1:T35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="P13" sqref="P13"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="12" max="12" width="13.6640625" customWidth="1"/>
-    <col min="13" max="13" width="10.33203125" customWidth="1"/>
-    <col min="19" max="19" width="23.109375" customWidth="1"/>
-    <col min="20" max="20" width="2.88671875" customWidth="1"/>
+    <col min="12" max="12" width="13.7109375" customWidth="1"/>
+    <col min="13" max="13" width="10.28515625" customWidth="1"/>
+    <col min="19" max="19" width="23.140625" customWidth="1"/>
+    <col min="20" max="20" width="2.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:20" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="16" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="16" t="s">
         <v>9</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="11" t="s">
+      <c r="K1" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="L1" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="M1" s="18" t="s">
+      <c r="M1" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="N1" s="17" t="s">
+      <c r="N1" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="O1" s="17"/>
-      <c r="P1" s="17" t="s">
+      <c r="O1" s="13"/>
+      <c r="P1" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="Q1" s="17"/>
-      <c r="S1" s="19" t="s">
+      <c r="Q1" s="13"/>
+      <c r="S1" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="T1" s="19"/>
-    </row>
-    <row r="2" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="10"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
+      <c r="T1" s="14"/>
+    </row>
+    <row r="2" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="17"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
       <c r="H2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="10"/>
+      <c r="I2" s="17"/>
       <c r="J2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="12"/>
-      <c r="L2" s="8"/>
-      <c r="M2" s="13" t="s">
+      <c r="K2" s="19"/>
+      <c r="L2" s="15"/>
+      <c r="M2" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="N2" s="16" t="s">
+      <c r="N2" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="O2" s="16" t="s">
+      <c r="O2" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="P2" s="16" t="s">
+      <c r="P2" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="Q2" s="16" t="s">
+      <c r="Q2" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="R2" s="16" t="s">
+      <c r="R2" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="S2" s="16" t="s">
+      <c r="S2" s="11" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>0</v>
       </c>
@@ -1863,31 +1868,31 @@
         <f>AVERAGE(B3,C3,D3,E3,F3,G3,H3,I3,J3,K3)</f>
         <v>1.2000000000000003E-3</v>
       </c>
-      <c r="M3" s="14">
+      <c r="M3" s="9">
         <v>0.15</v>
       </c>
-      <c r="N3" s="14">
+      <c r="N3" s="9">
         <v>0</v>
       </c>
-      <c r="O3" s="14">
+      <c r="O3" s="9">
         <v>0</v>
       </c>
-      <c r="P3" s="14">
+      <c r="P3" s="9">
         <v>0.25</v>
       </c>
-      <c r="Q3" s="14">
+      <c r="Q3" s="9">
         <v>1.2109000000000001</v>
       </c>
-      <c r="R3" s="15">
+      <c r="R3" s="10">
         <f>(Q3-O3)/(P3-N3)</f>
         <v>4.8436000000000003</v>
       </c>
-      <c r="S3" s="15">
+      <c r="S3" s="21">
         <f>((M3-O3)/R3)+N3</f>
         <v>3.0968700966223468E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>0.25</v>
       </c>
@@ -1925,31 +1930,31 @@
         <f t="shared" ref="L4:L35" si="0">AVERAGE(B4,C4,D4,E4,F4,G4,H4,I4,J4,K4)</f>
         <v>1.2109000000000001</v>
       </c>
-      <c r="M4" s="14">
+      <c r="M4" s="9">
         <v>0.67300000000000004</v>
       </c>
-      <c r="N4" s="14">
+      <c r="N4" s="9">
         <v>0</v>
       </c>
-      <c r="O4" s="14">
+      <c r="O4" s="9">
         <v>0</v>
       </c>
-      <c r="P4" s="14">
+      <c r="P4" s="9">
         <v>0.25</v>
       </c>
-      <c r="Q4" s="14">
+      <c r="Q4" s="9">
         <v>1.2109000000000001</v>
       </c>
-      <c r="R4" s="15">
+      <c r="R4" s="10">
         <f t="shared" ref="R4:R7" si="1">(Q4-O4)/(P4-N4)</f>
         <v>4.8436000000000003</v>
       </c>
-      <c r="S4" s="15">
+      <c r="S4" s="21">
         <f t="shared" ref="S4:S7" si="2">((M4-O4)/R4)+N4</f>
         <v>0.13894623833512262</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>0.5</v>
       </c>
@@ -1987,31 +1992,31 @@
         <f t="shared" si="0"/>
         <v>1.8544</v>
       </c>
-      <c r="M5" s="14">
+      <c r="M5" s="9">
         <v>1.52</v>
       </c>
-      <c r="N5" s="14">
+      <c r="N5" s="9">
         <v>0.25</v>
       </c>
-      <c r="O5" s="14">
+      <c r="O5" s="9">
         <v>1.2109000000000001</v>
       </c>
-      <c r="P5" s="14">
+      <c r="P5" s="9">
         <v>0.5</v>
       </c>
-      <c r="Q5" s="14">
+      <c r="Q5" s="9">
         <v>1.8544</v>
       </c>
-      <c r="R5" s="15">
+      <c r="R5" s="10">
         <f t="shared" si="1"/>
         <v>2.5739999999999998</v>
       </c>
-      <c r="S5" s="15">
+      <c r="S5" s="21">
         <f t="shared" si="2"/>
         <v>0.37008547008547005</v>
       </c>
     </row>
-    <row r="6" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>0.75</v>
       </c>
@@ -2049,31 +2054,31 @@
         <f t="shared" si="0"/>
         <v>2.1203000000000003</v>
       </c>
-      <c r="M6" s="14">
+      <c r="M6" s="9">
         <v>1.82</v>
       </c>
-      <c r="N6" s="14">
+      <c r="N6" s="9">
         <v>0.25</v>
       </c>
-      <c r="O6" s="14">
+      <c r="O6" s="9">
         <v>1.2109000000000001</v>
       </c>
-      <c r="P6" s="14">
+      <c r="P6" s="9">
         <v>0.5</v>
       </c>
-      <c r="Q6" s="14">
+      <c r="Q6" s="9">
         <v>1.8544</v>
       </c>
-      <c r="R6" s="15">
+      <c r="R6" s="10">
         <f t="shared" si="1"/>
         <v>2.5739999999999998</v>
       </c>
-      <c r="S6" s="15">
+      <c r="S6" s="21">
         <f t="shared" si="2"/>
         <v>0.48663558663558665</v>
       </c>
     </row>
-    <row r="7" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>1</v>
       </c>
@@ -2111,31 +2116,31 @@
         <f t="shared" si="0"/>
         <v>2.2173000000000003</v>
       </c>
-      <c r="M7" s="14">
+      <c r="M7" s="9">
         <v>2.2050000000000001</v>
       </c>
-      <c r="N7" s="14">
+      <c r="N7" s="9">
         <v>1.5</v>
       </c>
-      <c r="O7" s="14">
+      <c r="O7" s="9">
         <v>2.226</v>
       </c>
-      <c r="P7" s="14">
+      <c r="P7" s="9">
         <v>2</v>
       </c>
-      <c r="Q7" s="14">
+      <c r="Q7" s="9">
         <v>2.1112000000000002</v>
       </c>
-      <c r="R7" s="15">
+      <c r="R7" s="10">
         <f t="shared" si="1"/>
         <v>-0.22959999999999958</v>
       </c>
-      <c r="S7" s="15">
+      <c r="S7" s="21">
         <f t="shared" si="2"/>
         <v>1.5914634146341462</v>
       </c>
     </row>
-    <row r="8" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>1.5</v>
       </c>
@@ -2174,7 +2179,7 @@
         <v>2.226</v>
       </c>
     </row>
-    <row r="9" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>2</v>
       </c>
@@ -2213,7 +2218,7 @@
         <v>2.1112000000000002</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>2.5</v>
       </c>
@@ -2252,7 +2257,7 @@
         <v>1.9189000000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>3</v>
       </c>
@@ -2290,8 +2295,10 @@
         <f t="shared" si="0"/>
         <v>1.7707000000000002</v>
       </c>
-    </row>
-    <row r="12" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="Q11" s="9"/>
+      <c r="R11" s="20"/>
+    </row>
+    <row r="12" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>3.5</v>
       </c>
@@ -2329,8 +2336,10 @@
         <f t="shared" si="0"/>
         <v>1.6473000000000002</v>
       </c>
-    </row>
-    <row r="13" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="Q12" s="9"/>
+      <c r="R12" s="20"/>
+    </row>
+    <row r="13" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>4</v>
       </c>
@@ -2368,8 +2377,10 @@
         <f t="shared" si="0"/>
         <v>1.4994999999999998</v>
       </c>
-    </row>
-    <row r="14" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="Q13" s="9"/>
+      <c r="R13" s="20"/>
+    </row>
+    <row r="14" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>4.5</v>
       </c>
@@ -2407,8 +2418,10 @@
         <f t="shared" si="0"/>
         <v>1.3721000000000001</v>
       </c>
-    </row>
-    <row r="15" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="Q14" s="9"/>
+      <c r="R14" s="20"/>
+    </row>
+    <row r="15" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>5</v>
       </c>
@@ -2446,8 +2459,10 @@
         <f t="shared" si="0"/>
         <v>1.2754999999999999</v>
       </c>
-    </row>
-    <row r="16" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="Q15" s="9"/>
+      <c r="R15" s="20"/>
+    </row>
+    <row r="16" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>5.5</v>
       </c>
@@ -2486,7 +2501,7 @@
         <v>1.1695999999999998</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>6</v>
       </c>
@@ -2524,8 +2539,9 @@
         <f t="shared" si="0"/>
         <v>1.0760000000000001</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="Q17" s="9"/>
+    </row>
+    <row r="18" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>6.5</v>
       </c>
@@ -2563,8 +2579,9 @@
         <f t="shared" si="0"/>
         <v>0.99680000000000002</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="Q18" s="9"/>
+    </row>
+    <row r="19" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <v>7</v>
       </c>
@@ -2602,8 +2619,9 @@
         <f t="shared" si="0"/>
         <v>0.92379999999999995</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="Q19" s="9"/>
+    </row>
+    <row r="20" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
         <v>7.5</v>
       </c>
@@ -2641,8 +2659,9 @@
         <f t="shared" si="0"/>
         <v>0.84619999999999995</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="Q20" s="9"/>
+    </row>
+    <row r="21" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
         <v>8</v>
       </c>
@@ -2680,8 +2699,9 @@
         <f t="shared" si="0"/>
         <v>0.74409999999999998</v>
       </c>
-    </row>
-    <row r="22" spans="1:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="Q21" s="9"/>
+    </row>
+    <row r="22" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
         <v>8.5</v>
       </c>
@@ -2720,7 +2740,7 @@
         <v>0.71819999999999995</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
         <v>9</v>
       </c>
@@ -2759,7 +2779,7 @@
         <v>0.64649999999999996</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
         <v>9.5</v>
       </c>
@@ -2798,7 +2818,7 @@
         <v>0.59210000000000007</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
         <v>10.5</v>
       </c>
@@ -2837,7 +2857,7 @@
         <v>0.51920000000000011</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="3">
         <v>11</v>
       </c>
@@ -2876,7 +2896,7 @@
         <v>0.44290000000000002</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
         <v>12</v>
       </c>
@@ -2915,7 +2935,7 @@
         <v>0.35810000000000003</v>
       </c>
     </row>
-    <row r="28" spans="1:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="3">
         <v>13</v>
       </c>
@@ -2954,7 +2974,7 @@
         <v>0.33360000000000001</v>
       </c>
     </row>
-    <row r="29" spans="1:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="3">
         <v>14</v>
       </c>
@@ -2993,7 +3013,7 @@
         <v>0.27430000000000004</v>
       </c>
     </row>
-    <row r="30" spans="1:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="3">
         <v>15</v>
       </c>
@@ -3032,7 +3052,7 @@
         <v>0.21929999999999997</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="3">
         <v>16</v>
       </c>
@@ -3071,7 +3091,7 @@
         <v>0.20200000000000001</v>
       </c>
     </row>
-    <row r="32" spans="1:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="3">
         <v>17</v>
       </c>
@@ -3110,7 +3130,7 @@
         <v>0.17099999999999999</v>
       </c>
     </row>
-    <row r="33" spans="1:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="3">
         <v>18</v>
       </c>
@@ -3149,7 +3169,7 @@
         <v>0.1394</v>
       </c>
     </row>
-    <row r="34" spans="1:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="3">
         <v>19</v>
       </c>
@@ -3188,7 +3208,7 @@
         <v>0.10269999999999999</v>
       </c>
     </row>
-    <row r="35" spans="1:12" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="3">
         <v>20</v>
       </c>
@@ -3229,6 +3249,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
     <mergeCell ref="N1:O1"/>
     <mergeCell ref="P1:Q1"/>
     <mergeCell ref="S1:T1"/>
@@ -3236,12 +3262,6 @@
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="K1:K2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>